<commit_message>
fetched data from db and shown on frontend
</commit_message>
<xml_diff>
--- a/backend/train-details.xlsx
+++ b/backend/train-details.xlsx
@@ -1,41 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\railwayBooking\backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D92FB9B-466A-45B6-A916-0ADAAC42C82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Train Details" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+  <si>
+    <t>trainName</t>
+  </si>
+  <si>
+    <t>trainNumber</t>
+  </si>
+  <si>
+    <t>journeyDate</t>
+  </si>
+  <si>
+    <t>journeyTime</t>
+  </si>
+  <si>
+    <t>acCoaches</t>
+  </si>
+  <si>
+    <t>sleeperCoaches</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>stops</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>s1, s2, s3, s4</t>
+  </si>
+  <si>
+    <t>deset</t>
+  </si>
+  <si>
+    <t>[{"_id":"645660315a9a01a887b42118","stationName":"stname","arrivalTime":"attime","departureTime":"dpttime","duration":"dura"}]</t>
+  </si>
+  <si>
+    <t>[{"_id":"645660315a9a01a887b42119","stationName":"stname","arrivalTime":"attime","departureTime":"dpttime","duration":"dura"}]</t>
+  </si>
+  <si>
+    <t>[{"_id":"645660315a9a01a887b4211a","stationName":"stname","arrivalTime":"attime","departureTime":"dpttime","duration":"dura"}]</t>
+  </si>
+  <si>
+    <t>[{"_id":"645660315a9a01a887b4211b","stationName":"stname","arrivalTime":"attime","departureTime":"dpttime","duration":"dura"}]</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -73,6 +121,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,247 +453,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>trainName</v>
-      </c>
-      <c r="B1" t="str">
-        <v>trainNumber</v>
-      </c>
-      <c r="C1" t="str">
-        <v>journeyDate</v>
-      </c>
-      <c r="D1" t="str">
-        <v>journeyTime</v>
-      </c>
-      <c r="E1" t="str">
-        <v>acCoaches</v>
-      </c>
-      <c r="F1" t="str">
-        <v>sleeperCoaches</v>
-      </c>
-      <c r="G1" t="str">
-        <v>source</v>
-      </c>
-      <c r="H1" t="str">
-        <v>destination</v>
-      </c>
-      <c r="I1" t="str">
-        <v>stops</v>
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B2" t="str">
-        <v>1234</v>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D2" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E2" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F2" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I2" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"6455501891ac0cbc4a2e0fde"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"6455501891ac0cbc4a2e0fdf"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"6455501891ac0cbc4a2e0fe0"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"6455501891ac0cbc4a2e0fe1"}]</v>
+        <v>45204.000115740739</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1234</v>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D3" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E3" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F3" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I3" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"6455501b27edd34b1d9f8be7"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"6455501b27edd34b1d9f8be8"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"6455501b27edd34b1d9f8be9"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"6455501b27edd34b1d9f8bea"}]</v>
+        <v>45204.000115740739</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B4" t="str">
-        <v>1234</v>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D4" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E4" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F4" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I4" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"6455501db7452f2abe3cbeb6"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"6455501db7452f2abe3cbeb7"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"6455501db7452f2abe3cbeb8"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"6455501db7452f2abe3cbeb9"}]</v>
+        <v>45204.000115740739</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B5" t="str">
-        <v>1234</v>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D5" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E5" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F5" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I5" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"64555021c3c98040d7e31095"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"64555021c3c98040d7e31096"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"64555021c3c98040d7e31097"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"64555021c3c98040d7e31098"}]</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B6" t="str">
-        <v>1234</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D6" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E6" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F6" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I6" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"64555029cdd03435792ff4dc"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"64555029cdd03435792ff4dd"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"64555029cdd03435792ff4de"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"64555029cdd03435792ff4df"}]</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B7" t="str">
-        <v>1234</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D7" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E7" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F7" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I7" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"6455502dfce78fc9a9a1e39b"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"6455502dfce78fc9a9a1e39c"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"6455502dfce78fc9a9a1e39d"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"6455502dfce78fc9a9a1e39e"}]</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Rajdhani Express</v>
-      </c>
-      <c r="B8" t="str">
-        <v>1234</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45056.22928240741</v>
-      </c>
-      <c r="D8" t="str">
-        <v>8:00 AM</v>
-      </c>
-      <c r="E8" t="str">
-        <v>A1, A2, A3</v>
-      </c>
-      <c r="F8" t="str">
-        <v>S1, S2, S3</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Delhi</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Mumbai</v>
-      </c>
-      <c r="I8" t="str">
-        <v>[{"stationName":"Jaipur","arrivalTime":"11:00 AM","departureTime":"11:10 AM","duration":"10 minutes","_id":"64555040ee543607715e6c1a"},{"stationName":"Ahmedabad","arrivalTime":"2:00 PM","departureTime":"2:15 PM","duration":"15 minutes","_id":"64555040ee543607715e6c1b"},{"stationName":"Surat","arrivalTime":"5:00 PM","departureTime":"5:05 PM","duration":"5 minutes","_id":"64555040ee543607715e6c1c"},{"stationName":"Vadodara","arrivalTime":"4:00 PM","departureTime":"4:10 PM","duration":"10 minutes","_id":"64555040ee543607715e6c1d"}]</v>
+        <v>45204.000115740739</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I8"/>
+    <ignoredError sqref="A1:I1 A3:I5 A2:D2 F2:I2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>